<commit_message>
updated offshore wind limit
</commit_message>
<xml_diff>
--- a/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
+++ b/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\elec\MPCbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5077E0-1E7A-4F94-A974-B998BDE33BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857A4070-2693-4133-8526-4EA142A27361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15195" yWindow="1020" windowWidth="12585" windowHeight="13980" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="75" windowWidth="14700" windowHeight="16200" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="239">
   <si>
     <t>MPCbS Max Potential Capacity by Source</t>
   </si>
@@ -756,6 +756,9 @@
   </si>
   <si>
     <t>CEC</t>
+  </si>
+  <si>
+    <t>build 10GW in BPMCCS, assume 21-10 is potential</t>
   </si>
 </sst>
 </file>
@@ -1147,6 +1150,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1"/>
@@ -1164,8 +1169,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7370,54 +7373,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="56"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="8">
         <v>2020</v>
       </c>
@@ -8737,11 +8740,11 @@
       <c r="J56" s="16"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="55" t="s">
+      <c r="A57" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="B57" s="56"/>
-      <c r="C57" s="56"/>
+      <c r="B57" s="58"/>
+      <c r="C57" s="58"/>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
       <c r="F57" s="16"/>
@@ -8765,35 +8768,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E6CB4D-7EA0-407B-BC73-DE2B39553891}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="55" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="55" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="55" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="65">
+      <c r="A4" s="56">
         <v>44687</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="55" t="s">
         <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -8941,8 +8951,8 @@
         <v>163</v>
       </c>
       <c r="B14" s="9">
-        <f>21.8*1000</f>
-        <v>21800</v>
+        <f>(21.8*1000)-10000</f>
+        <v>11800</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -15101,18 +15111,18 @@
     </row>
     <row r="3" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="32"/>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="63" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="65"/>
       <c r="M3" s="27" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Revert "updated offshore wind limit"
This reverts commit f43bfc9b3eb3cc8f106cf825ec77ef6ce7907405.
</commit_message>
<xml_diff>
--- a/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
+++ b/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\elec\MPCbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857A4070-2693-4133-8526-4EA142A27361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5077E0-1E7A-4F94-A974-B998BDE33BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="75" windowWidth="14700" windowHeight="16200" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15195" yWindow="1020" windowWidth="12585" windowHeight="13980" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="238">
   <si>
     <t>MPCbS Max Potential Capacity by Source</t>
   </si>
@@ -756,9 +756,6 @@
   </si>
   <si>
     <t>CEC</t>
-  </si>
-  <si>
-    <t>build 10GW in BPMCCS, assume 21-10 is potential</t>
   </si>
 </sst>
 </file>
@@ -1150,8 +1147,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1"/>
@@ -1169,6 +1164,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7373,54 +7370,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="58"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="56"/>
       <c r="C4" s="8">
         <v>2020</v>
       </c>
@@ -8740,11 +8737,11 @@
       <c r="J56" s="16"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="57" t="s">
+      <c r="A57" s="55" t="s">
         <v>148</v>
       </c>
-      <c r="B57" s="58"/>
-      <c r="C57" s="58"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="56"/>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
       <c r="F57" s="16"/>
@@ -8768,42 +8765,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E6CB4D-7EA0-407B-BC73-DE2B39553891}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="64" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="64" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="64" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="56">
+      <c r="A4" s="65">
         <v>44687</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="64" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -8951,8 +8941,8 @@
         <v>163</v>
       </c>
       <c r="B14" s="9">
-        <f>(21.8*1000)-10000</f>
-        <v>11800</v>
+        <f>21.8*1000</f>
+        <v>21800</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -15111,18 +15101,18 @@
     </row>
     <row r="3" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="32"/>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="65"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="63"/>
       <c r="M3" s="27" t="s">
         <v>2</v>
       </c>

</xml_diff>